<commit_message>
se realizo la clase de formulas financieras
</commit_message>
<xml_diff>
--- a/2015-2016/clases/computacion_aplicada_2/evaluacion.xlsx
+++ b/2015-2016/clases/computacion_aplicada_2/evaluacion.xlsx
@@ -379,8 +379,8 @@
   </sheetPr>
   <dimension ref="B4:N33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -476,9 +476,11 @@
       <c r="C8" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="N8" s="4" t="e">
+      <c r="N8" s="4" t="inlineStr">
         <f aca="false">AVERAGE(D8:M8)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -536,6 +538,9 @@
       <c r="D12" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="E12" s="0" t="n">
+        <v>10</v>
+      </c>
       <c r="N12" s="4" t="n">
         <f aca="false">AVERAGE(D12:M12)*15/10</f>
         <v>15</v>
@@ -578,9 +583,11 @@
       <c r="C15" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="N15" s="4" t="e">
+      <c r="N15" s="4" t="inlineStr">
         <f aca="false">AVERAGE(D15:M15)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -620,9 +627,11 @@
       <c r="C18" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="N18" s="4" t="e">
+      <c r="N18" s="4" t="inlineStr">
         <f aca="false">AVERAGE(D18:M18)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -665,9 +674,12 @@
       <c r="D21" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="E21" s="0" t="n">
+        <v>10</v>
+      </c>
       <c r="N21" s="4" t="n">
         <f aca="false">AVERAGE(D21:M21)*15/10</f>
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -725,9 +737,11 @@
       <c r="C25" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="N25" s="4" t="e">
+      <c r="N25" s="4" t="inlineStr">
         <f aca="false">AVERAGE(D25:M25)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>